<commit_message>
Added information about box mass
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -16,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,6 +27,7 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,15 +45,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="datetime" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,32 +466,117 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>Displaced</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>Elements</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>NAtoms</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Bad</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Duration</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>AlphaCount</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Filename</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>RunNumber</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Dead_0</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Dead_1</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>BaCorr_0</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>BaCorr_0_err</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>BaCorr_1</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>BaCorr_1_err</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>BaCorr_2</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>BaCorr_2_err</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>BaCorr_3</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>BaCorr_3_err</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>BaCorr_4</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>BaCorr_4_err</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>BaCorr_5</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>BaCorr_5_err</t>
         </is>
       </c>
     </row>
@@ -516,29 +608,82 @@
           <t>[343.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>[Sn]</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
         <v>10512</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>5188779524</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>test182_HPGe_2_Labr_4_Ing27_80prc_Generator_100hz_Ba_center_Pb_1mm_Sn_1cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O2" t="n">
+        <v>182</v>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>26/11/2024</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.8779855152364474</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.8756789525079685</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.194166235012017</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.01479099974266805</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1.240896382247949</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.01172870661554532</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9470321562816976</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.01703966834059936</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9780950383557171</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.00957309707929623</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.9627019987300519</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.01132485525432071</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8983120454031256</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.01565113013559638</v>
       </c>
     </row>
     <row r="3">
@@ -561,7 +706,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -569,29 +714,82 @@
           <t>[366.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>[Ti,O]</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
         <v>14400</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>8207514617</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>test148_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_TiO2_4cm.root</t>
         </is>
+      </c>
+      <c r="O3" t="n">
+        <v>148</v>
+      </c>
+      <c r="P3" s="1" t="inlineStr">
+        <is>
+          <t>05/08/2024</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.8625899116126892</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.861920552892728</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1.393412588880313</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.01599272252519878</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1.246081653956609</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0.01986758119929219</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1.080371071540968</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.005437383006366726</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1.011139906304793</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.006635286286346161</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1.083710637029356</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.009756686333953848</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.988000055178012</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>0.01076488459276884</v>
       </c>
     </row>
     <row r="4">
@@ -614,7 +812,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -622,29 +820,82 @@
           <t>[366.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>[Al,O]</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>[2,3]</t>
         </is>
       </c>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
         <v>14400</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>7980344770</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>test153_HPGe_2_Labr_4_Ing27_81prc_Generator_100hz_Ba_center_Pb_1mm_Al2O3_4cm.root</t>
         </is>
+      </c>
+      <c r="O4" t="n">
+        <v>153</v>
+      </c>
+      <c r="P4" s="1" t="inlineStr">
+        <is>
+          <t>07/08/2024</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.8621030517839643</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.8595056304673108</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1.369881616837573</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.01590864145639783</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1.237249023537758</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.02048187383127233</v>
+      </c>
+      <c r="W4" t="n">
+        <v>1.075842244180675</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.0059870966912306</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>1.004852065639871</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.006913844534266818</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1.061107318277587</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.008902030545068136</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.9740081462591751</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0.01015274530217595</v>
       </c>
     </row>
     <row r="5">
@@ -675,29 +926,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>[K,Cl]</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>14400</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>7911647982</v>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>test177_HPGe_2_Labr_4_Ing27_80prc_Generator_100hz_Ba_center_Pb_1mm_KCl_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O5" t="n">
+        <v>177</v>
+      </c>
+      <c r="P5" s="1" t="inlineStr">
+        <is>
+          <t>19/11/2024</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.8590140856787761</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.8613977923673138</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.204761349779079</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.01634108666209831</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1.262885258704878</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.01314811178704073</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1.019359667527189</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.007070375892666369</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.9967754763395562</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.008543850236165067</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1.071752706378638</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.007710925400438469</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.9310073842657681</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0.0101704484040255</v>
       </c>
     </row>
     <row r="6">
@@ -720,7 +1024,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -728,29 +1032,46 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>[Cr,O]</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>[2,3]</t>
         </is>
       </c>
-      <c r="J6" t="b">
+      <c r="K6" t="b">
         <v>1</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>32000</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>7350591870</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>test152_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_Cr2O3_2cm.root</t>
         </is>
+      </c>
+      <c r="O6" t="n">
+        <v>152</v>
+      </c>
+      <c r="P6" s="1" t="inlineStr">
+        <is>
+          <t>06/08/2024</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.9363340605267656</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.9378197194392813</v>
       </c>
     </row>
     <row r="7">
@@ -773,7 +1094,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -781,29 +1102,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>[Cu]</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
         <v>14400</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>8957161477</v>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>test158_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_Cu_2cm.root</t>
         </is>
+      </c>
+      <c r="O7" t="n">
+        <v>158</v>
+      </c>
+      <c r="P7" s="1" t="inlineStr">
+        <is>
+          <t>09/08/2024</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.8499532889329947</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.8470378986422333</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1.410229648113126</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.02906805636075532</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1.249280060667686</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.0338014752890502</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1.194855776868655</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.006749504945041312</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1.119713146906225</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.00806671034082519</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>1.171102250462451</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.01006286202156612</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>1.026868764744553</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.01332267704364146</v>
       </c>
     </row>
     <row r="8">
@@ -834,29 +1208,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>[Be,O]</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
         <v>28800</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>15154449901</v>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>test180_HPGe_2_Labr_4_Ing27_83prc_Generator_100hz_Ba_center_Pb_1mm_BeO_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O8" t="n">
+        <v>180</v>
+      </c>
+      <c r="P8" s="1" t="inlineStr">
+        <is>
+          <t>25/11/2024</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.8641033049595842</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.8682813248446919</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1.196183625978048</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.01564427264486803</v>
+      </c>
+      <c r="U8" t="n">
+        <v>1.293186079840831</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.00986610138033385</v>
+      </c>
+      <c r="W8" t="n">
+        <v>1.052189210954905</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.006458943301756736</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.9801472865930696</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.00671694777256869</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1.051801397439637</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.007618140598867311</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.9031061248431139</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.01257100874056446</v>
       </c>
     </row>
     <row r="9">
@@ -879,7 +1306,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -887,29 +1314,82 @@
           <t>[366.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>[Ca,O]</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
         <v>14400</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>8429087747</v>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>test155_HPGe_2_Labr_4_Ing27_81prc_Generator_100hz_Ba_center_Pb_1mm_CaO_4cm.root</t>
         </is>
+      </c>
+      <c r="O9" t="n">
+        <v>155</v>
+      </c>
+      <c r="P9" s="1" t="inlineStr">
+        <is>
+          <t>08/08/2024</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.8636034636880906</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.8591581403494689</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.8198454850622254</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.009986000754233917</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.7388208700455674</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.01244452824098883</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.619811419808375</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.00580541773332953</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.5744612362353309</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.007820188028006214</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.6245576978740667</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.007587204462157892</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.6012699232343751</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.01291688498386284</v>
       </c>
     </row>
     <row r="10">
@@ -940,29 +1420,82 @@
           <t>[343.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>[Sn]</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
         <v>3034</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>1649123966</v>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>test184_HPGe_2_Labr_4_Ing27_85prc_Generator_100hz_Ba_center_Pb_1mm_Sn_1cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O10" t="n">
+        <v>184</v>
+      </c>
+      <c r="P10" s="1" t="inlineStr">
+        <is>
+          <t>28/11/2024</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.8660691370058905</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.8651942210788937</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1.214539093266109</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.01925702148395117</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1.262922334281536</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.0134889623361661</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.9689912694493901</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.01080093706369524</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.9729111324133363</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.01292165167834948</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.9593942821276971</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.01487037777930572</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.8931974541054146</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.01770854433856761</v>
       </c>
     </row>
     <row r="11">
@@ -993,29 +1526,46 @@
           <t>[348.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>[0,]</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>[0,0]</t>
         </is>
       </c>
-      <c r="J11" t="b">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
         <v>7266</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>4579201966</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>test147_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_Box_2cm.root</t>
         </is>
+      </c>
+      <c r="O11" t="n">
+        <v>147</v>
+      </c>
+      <c r="P11" s="1" t="inlineStr">
+        <is>
+          <t>24/07/2024</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.8487266326635792</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.8556639340738162</v>
       </c>
     </row>
     <row r="12">
@@ -1038,7 +1588,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1046,29 +1596,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>[Si,O]</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>[1,2]</t>
         </is>
       </c>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>10400</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>6319447173</v>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>test159_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_SiO2_2cm.root</t>
         </is>
+      </c>
+      <c r="O12" t="n">
+        <v>159</v>
+      </c>
+      <c r="P12" s="1" t="inlineStr">
+        <is>
+          <t>09/08/2024</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.8519693307280658</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.8482341783010161</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1.459262957611143</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.01335654753186675</v>
+      </c>
+      <c r="U12" t="n">
+        <v>1.256907175276956</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.0223367731171598</v>
+      </c>
+      <c r="W12" t="n">
+        <v>1.110595828326371</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.006085735314830268</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>1.031400545373676</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.007756053574967812</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>1.08052898613157</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.008012267175951906</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.9570326347583266</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.01132815094271584</v>
       </c>
     </row>
     <row r="13">
@@ -1099,29 +1702,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>[B,N]</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
+      <c r="K13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
         <v>8628</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>4613160753</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>test173_HPGe_2_Labr_4_Ing27_83prc_Generator_100hz_Ba_center_Pb_1mm_BN_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O13" t="n">
+        <v>173</v>
+      </c>
+      <c r="P13" s="1" t="inlineStr">
+        <is>
+          <t>12/11/2024</t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.85439788248481</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.8660106005283802</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1.399479544699705</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.01811975148347007</v>
+      </c>
+      <c r="U13" t="n">
+        <v>1.205677433662329</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.02549820736955906</v>
+      </c>
+      <c r="W13" t="n">
+        <v>1.012632974407412</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.006956307662208668</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.9513527559195523</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.01362493468860575</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>1.090236235450669</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.00937956266835952</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.898185864394504</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.01274755600943568</v>
       </c>
     </row>
     <row r="14">
@@ -1152,29 +1808,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>[S]</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
         <v>14400</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>8004943205</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>test179_HPGe_2_Labr_4_Ing27_81prc_Generator_100hz_Ba_center_Pb_1mm_S_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O14" t="n">
+        <v>179</v>
+      </c>
+      <c r="P14" s="1" t="inlineStr">
+        <is>
+          <t>20/11/2024</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.8576229957594406</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.8563199973450614</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1.220653327925448</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.01709540364284433</v>
+      </c>
+      <c r="U14" t="n">
+        <v>1.285972182430215</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.0160444604848006</v>
+      </c>
+      <c r="W14" t="n">
+        <v>1.006365332587891</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.007070821508370581</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.9894278991537435</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.008363423210158632</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>1.051900668969805</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0.008255708250342466</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0.932580515407049</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.01135066962366682</v>
       </c>
     </row>
     <row r="15">
@@ -1205,29 +1914,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>[Mg,O]</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
         <v>14400</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>7884387338</v>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>test185_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_MgO_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O15" t="n">
+        <v>185</v>
+      </c>
+      <c r="P15" s="1" t="inlineStr">
+        <is>
+          <t>29/11/2024</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.8613569948377732</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.8594523672860086</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1.237570217605701</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.04249442369337261</v>
+      </c>
+      <c r="U15" t="n">
+        <v>1.37421028571625</v>
+      </c>
+      <c r="V15" t="n">
+        <v>0.02664068234624344</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1.109805959204139</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.007880831270791084</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>1.075189429797333</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.009187223851566709</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>1.138671964573963</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0.007311295682635487</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0.996466985962513</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.01264794635420997</v>
       </c>
     </row>
     <row r="16">
@@ -1258,29 +2020,82 @@
           <t>[348.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>[Si,O]</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>[1,2]</t>
         </is>
       </c>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
         <v>4004</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>2628009168</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>test146_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_SiO2.root</t>
         </is>
+      </c>
+      <c r="O16" t="n">
+        <v>146</v>
+      </c>
+      <c r="P16" s="1" t="inlineStr">
+        <is>
+          <t>24/07/2024</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.8361015225403793</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.844570362511192</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.33193796206688</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.02219682500749243</v>
+      </c>
+      <c r="U16" t="n">
+        <v>1.192530329414469</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.02134525160577657</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.9260786481877973</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.00836149422992641</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.865334938150765</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.009630328597678775</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1.048681556671274</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0.0110140204778421</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0.9326294338165438</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.01445962185616215</v>
       </c>
     </row>
     <row r="17">
@@ -1311,29 +2126,46 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>[B,N]</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J17" t="b">
+      <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>7816</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>4814438573</v>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="N17" t="inlineStr">
         <is>
           <t>test172_HPGe_2_Labr_4_Ing27_83prc_Generator_100hz_Ba_center_Pb_1mm_BN_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O17" t="n">
+        <v>172</v>
+      </c>
+      <c r="P17" s="1" t="inlineStr">
+        <is>
+          <t>12/11/2024</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.8401048261746129</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.84846574544873</v>
       </c>
     </row>
     <row r="18">
@@ -1356,7 +2188,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1364,29 +2196,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>[Cr,O]</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>[2,3]</t>
         </is>
       </c>
-      <c r="J18" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
         <v>2972</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>1959093786</v>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>test149_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_Cr2O3_2cm.root</t>
         </is>
+      </c>
+      <c r="O18" t="n">
+        <v>149</v>
+      </c>
+      <c r="P18" s="1" t="inlineStr">
+        <is>
+          <t>29/11/2024</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.8412943626300826</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.8403667451154621</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1.495461740179218</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.02243415307286464</v>
+      </c>
+      <c r="U18" t="n">
+        <v>1.323109301232849</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0.02509571508150587</v>
+      </c>
+      <c r="W18" t="n">
+        <v>1.142219719321269</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.009829567273926297</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>1.057441014734345</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.01215934316493628</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>1.142911750642372</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0.01309501673745081</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>0.9923680416490718</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.01533015478775306</v>
       </c>
     </row>
     <row r="19">
@@ -1409,7 +2294,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1417,29 +2302,46 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>[Cr,O]</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>[2,3]</t>
         </is>
       </c>
-      <c r="J19" t="b">
+      <c r="K19" t="b">
         <v>1</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>2828</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>2929855911</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>test150_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_Cr2O3_2cm.root</t>
         </is>
+      </c>
+      <c r="O19" t="n">
+        <v>150</v>
+      </c>
+      <c r="P19" s="1" t="inlineStr">
+        <is>
+          <t>06/08/2024</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.753306649050304</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.7539056101180558</v>
       </c>
     </row>
     <row r="20">
@@ -1462,7 +2364,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1470,29 +2372,82 @@
           <t>[366.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>[Na,O,H]</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>[1,1,1]</t>
         </is>
       </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
         <v>15088</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>8719768937</v>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>test154_HPGe_2_Labr_4_Ing27_81prc_Generator_100hz_Ba_center_Pb_1mm_NaOH_4cm.root</t>
         </is>
+      </c>
+      <c r="O20" t="n">
+        <v>154</v>
+      </c>
+      <c r="P20" s="1" t="inlineStr">
+        <is>
+          <t>07/08/2024</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.8574658057201389</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.8546054902692568</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1.406972924941439</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.01482933437122944</v>
+      </c>
+      <c r="U20" t="n">
+        <v>1.256338842395359</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.02182565375217692</v>
+      </c>
+      <c r="W20" t="n">
+        <v>1.037105456014566</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.006465714291562492</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.9832134884136927</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.007863814137966958</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0.9553099614877548</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0.0078299932340561</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>0.9259338002405808</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.01197768689478693</v>
       </c>
     </row>
     <row r="21">
@@ -1515,7 +2470,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1523,29 +2478,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>[Mn,O]</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>[1,2]</t>
         </is>
       </c>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
         <v>14400</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>8779992270</v>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>test160_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_Mn2O3_2cm.root</t>
         </is>
+      </c>
+      <c r="O21" t="n">
+        <v>160</v>
+      </c>
+      <c r="P21" s="1" t="inlineStr">
+        <is>
+          <t>23/08/2024</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.8563190668244465</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.8522859923522096</v>
+      </c>
+      <c r="S21" t="n">
+        <v>1.42132056184074</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.01455506713762738</v>
+      </c>
+      <c r="U21" t="n">
+        <v>1.280266501536245</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.02232653484942316</v>
+      </c>
+      <c r="W21" t="n">
+        <v>1.101546625733805</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0.005476521441732364</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>1.042051833698277</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.006754997126191271</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>1.076751331662246</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0.008013091624593908</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0.9948484175184567</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.009549785856286908</v>
       </c>
     </row>
     <row r="22">
@@ -1576,29 +2584,46 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>[P,O]</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>[2,5]</t>
         </is>
       </c>
-      <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
         <v>13704</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>6868758348</v>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="N22" t="inlineStr">
         <is>
           <t>test186_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_P2O5_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O22" t="n">
+        <v>186</v>
+      </c>
+      <c r="P22" s="1" t="inlineStr">
+        <is>
+          <t>04/12/2024</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.8734184631234843</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.8696555685888919</v>
       </c>
     </row>
     <row r="23">
@@ -1629,29 +2654,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>[C,H,Cl]</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>[1,2,2]</t>
         </is>
       </c>
-      <c r="J23" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
         <v>14400</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>7720079428</v>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="N23" t="inlineStr">
         <is>
           <t>test161_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_CH2Cl2_4cm.root</t>
         </is>
+      </c>
+      <c r="O23" t="n">
+        <v>161</v>
+      </c>
+      <c r="P23" s="1" t="inlineStr">
+        <is>
+          <t>25/08/2024</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.8872821996461518</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.8795517260820696</v>
+      </c>
+      <c r="S23" t="n">
+        <v>1.378930000644863</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.01390240739474842</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1.198256557809707</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0.02058223922595847</v>
+      </c>
+      <c r="W23" t="n">
+        <v>1.049485019698752</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0.005702656043627607</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0.9961401056203174</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0.006191209273978928</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>1.064232977327821</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0.007952746833509914</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0.9549853744638505</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0.01150052511870442</v>
       </c>
     </row>
     <row r="24">
@@ -1682,29 +2760,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>[Na,Cl]</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J24" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
         <v>14400</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>7831675309</v>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="N24" t="inlineStr">
         <is>
           <t>test176_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_NaCl_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O24" t="n">
+        <v>176</v>
+      </c>
+      <c r="P24" s="1" t="inlineStr">
+        <is>
+          <t>18/11/2024</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.8578197973521374</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.85875752613359</v>
+      </c>
+      <c r="S24" t="n">
+        <v>1.207606799118192</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.01843274687620216</v>
+      </c>
+      <c r="U24" t="n">
+        <v>1.244299785601783</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.02037104369792916</v>
+      </c>
+      <c r="W24" t="n">
+        <v>1.005256427644023</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.006346104172057787</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.9800651231859338</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.008488512655443464</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>1.066497242068614</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0.008660520185145784</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.9022542926478716</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0.01165837286367675</v>
       </c>
     </row>
     <row r="25">
@@ -1735,29 +2866,82 @@
           <t>[343.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>[Sn]</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" t="n">
         <v>10512</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>5188779524</v>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="N25" t="inlineStr">
         <is>
           <t>test182_HPGe_2_Labr_4_Ing27_85prc_Generator_100hz_Ba_center_Pb_1mm_Sn_1cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O25" t="n">
+        <v>182</v>
+      </c>
+      <c r="P25" s="1" t="inlineStr">
+        <is>
+          <t>26/11/2024</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.8779558042178432</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.8756751438932341</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1.194261913935201</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.01457613196728747</v>
+      </c>
+      <c r="U25" t="n">
+        <v>1.240804555881466</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.01200415890835918</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.9464883333360088</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.01697811213819002</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0.9780314906237428</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0.009605027286460356</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0.9625719771080766</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0.01115239562392788</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0.8983123354254799</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0.01570310843238492</v>
       </c>
     </row>
     <row r="26">
@@ -1788,29 +2972,82 @@
           <t>[343.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>[Sn]</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J26" t="b">
+      <c r="K26" t="b">
         <v>1</v>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>1002</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>721297713</v>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="N26" t="inlineStr">
         <is>
           <t>test183_HPGe_2_Labr_4_Ing27_80prc_Generator_100hz_Ba_center_Pb_1mm_Sn_1cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O26" t="n">
+        <v>183</v>
+      </c>
+      <c r="P26" s="1" t="inlineStr">
+        <is>
+          <t>28/11/2024</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.8226023821319457</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.8241623418040649</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1.31967505562609</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0.02745246339964923</v>
+      </c>
+      <c r="U26" t="n">
+        <v>1.378286387475662</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.02396016291559647</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.506003167442958</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0.1060571725337814</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.9331715246794371</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0.05492043902664669</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>0.7207800077106851</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0.06491157374657222</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0.7712626904391741</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0.04996014685177066</v>
       </c>
     </row>
     <row r="27">
@@ -1841,29 +3078,46 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>[B,N]</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J27" t="b">
+      <c r="K27" t="b">
         <v>1</v>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>6762</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>3674070799</v>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="N27" t="inlineStr">
         <is>
           <t>test171_HPGe_2_Labr_4_Ing27_83prc_Generator_100hz_Ba_center_Pb_1mm_BN_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O27" t="n">
+        <v>171</v>
+      </c>
+      <c r="P27" s="1" t="inlineStr">
+        <is>
+          <t>11/11/2024</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.8596924156496923</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.8638542198906388</v>
       </c>
     </row>
     <row r="28">
@@ -1886,7 +3140,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1894,29 +3148,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>[Ni,O]</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>[2,3]</t>
         </is>
       </c>
-      <c r="J28" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
         <v>14400</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>8648486289</v>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="N28" t="inlineStr">
         <is>
           <t>test157_HPGe_2_Labr_4_Ing27_86prc_Generator_100hz_Ba_center_Pb_1mm_NiO_2cm.root</t>
         </is>
+      </c>
+      <c r="O28" t="n">
+        <v>157</v>
+      </c>
+      <c r="P28" s="1" t="inlineStr">
+        <is>
+          <t>08/08/2024</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.8540253386717347</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.8506940948059497</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1.42513221130806</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.01830283355575749</v>
+      </c>
+      <c r="U28" t="n">
+        <v>1.241794507462411</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.0227108895672816</v>
+      </c>
+      <c r="W28" t="n">
+        <v>1.096122651196176</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0.006042061696325405</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>1.034075306779522</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0.00674617460461214</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>1.075465180814702</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0.010184880625068</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.9668151849694828</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.0121659676723224</v>
       </c>
     </row>
     <row r="29">
@@ -1939,7 +3246,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1947,29 +3254,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>[Cr,O]</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>[2,3]</t>
         </is>
       </c>
-      <c r="J29" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" t="n">
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
         <v>1624</v>
       </c>
-      <c r="L29" t="n">
+      <c r="M29" t="n">
         <v>1033300081</v>
       </c>
-      <c r="M29" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>test151_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_Cr2O3_2cm.root</t>
         </is>
+      </c>
+      <c r="O29" t="n">
+        <v>151</v>
+      </c>
+      <c r="P29" s="1" t="inlineStr">
+        <is>
+          <t>06/08/2024</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.8451951564308383</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.8425486043458766</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1.467167214559873</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.02261537483401699</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1.296413567175442</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.02176919579830242</v>
+      </c>
+      <c r="W29" t="n">
+        <v>1.120949185550618</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0.01033756920201833</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>1.027671795463382</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0.01335733276311759</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>1.10047818745739</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0.01376455745609188</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0.9762140424271077</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0.01912178489756006</v>
       </c>
     </row>
     <row r="30">
@@ -2000,29 +3360,82 @@
           <t>[348.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>[Zn]</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J30" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" t="n">
+      <c r="K30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
         <v>14400</v>
       </c>
-      <c r="L30" t="n">
+      <c r="M30" t="n">
         <v>8991743393</v>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>test169_HPGe_2_Labr_4_Ing27_82prc_Generator_100hz_Ba_center_Pb_1mm_Zn_2cm.root</t>
         </is>
+      </c>
+      <c r="O30" t="n">
+        <v>169</v>
+      </c>
+      <c r="P30" s="1" t="inlineStr">
+        <is>
+          <t>29/08/2024</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.8474900227657264</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.8435600163414251</v>
+      </c>
+      <c r="S30" t="n">
+        <v>1.401794533309768</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.01690558428957598</v>
+      </c>
+      <c r="U30" t="n">
+        <v>1.262345145959561</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.02339046218052609</v>
+      </c>
+      <c r="W30" t="n">
+        <v>1.010804237724272</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0.01167571314807085</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.991524716728673</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0.008656335008538525</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>1.062638677269736</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0.009086372680981995</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0.9847362475574458</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0.01122360834564715</v>
       </c>
     </row>
     <row r="31">
@@ -2053,29 +3466,82 @@
           <t>[348.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>[Co,O]</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="J31" t="inlineStr">
         <is>
           <t>[3,4]</t>
         </is>
       </c>
-      <c r="J31" t="b">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" t="n">
         <v>14400</v>
       </c>
-      <c r="L31" t="n">
+      <c r="M31" t="n">
         <v>7334299270</v>
       </c>
-      <c r="M31" t="inlineStr">
+      <c r="N31" t="inlineStr">
         <is>
           <t>test181_HPGe_2_Labr_4_Ing27_85prc_Generator_100hz_Ba_center_Pb_1mm_Co3O4_2cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O31" t="n">
+        <v>181</v>
+      </c>
+      <c r="P31" s="1" t="inlineStr">
+        <is>
+          <t>26/11/2024</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.8727254644833771</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.8711775813467613</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1.174258909066694</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.01524697711295829</v>
+      </c>
+      <c r="U31" t="n">
+        <v>1.251122076309749</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.01205986419998925</v>
+      </c>
+      <c r="W31" t="n">
+        <v>1.021852491714621</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0.007488705330853165</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.9886999477279934</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0.01108112191498567</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>1.060073256866571</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.008496379154197334</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.9269649561915387</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.01097674057944936</v>
       </c>
     </row>
     <row r="32">
@@ -2106,29 +3572,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>[Li,F]</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J32" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" t="n">
         <v>14400</v>
       </c>
-      <c r="L32" t="n">
+      <c r="M32" t="n">
         <v>9060719449</v>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>test170_HPGe_2_Labr_4_Ing27_87prc_Generator_100hz_Ba_center_Pb_1mm_LiF_4cm.root</t>
         </is>
+      </c>
+      <c r="O32" t="n">
+        <v>170</v>
+      </c>
+      <c r="P32" s="1" t="inlineStr">
+        <is>
+          <t>30/08/2024</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.843820520495285</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.8347335069197406</v>
+      </c>
+      <c r="S32" t="n">
+        <v>1.457147631936784</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.016268535463019</v>
+      </c>
+      <c r="U32" t="n">
+        <v>1.259025688952275</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.02426887191844622</v>
+      </c>
+      <c r="W32" t="n">
+        <v>1.043681358328096</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.007156474483538415</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1.022299299442683</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.00781634309514573</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>1.074632970021531</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0.00944619004303017</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.9838705994983694</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.01230741483860992</v>
       </c>
     </row>
     <row r="33">
@@ -2159,29 +3678,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>[V,O]</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>[2,5]</t>
         </is>
       </c>
-      <c r="J33" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
         <v>14400</v>
       </c>
-      <c r="L33" t="n">
+      <c r="M33" t="n">
         <v>7503692508</v>
       </c>
-      <c r="M33" t="inlineStr">
+      <c r="N33" t="inlineStr">
         <is>
           <t>test178_HPGe_2_Labr_4_Ing27_84prc_Generator_100hz_Ba_center_Pb_1mm_V2O5_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O33" t="n">
+        <v>178</v>
+      </c>
+      <c r="P33" s="1" t="inlineStr">
+        <is>
+          <t>20/11/2024</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.8670932859325857</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.8692601126826335</v>
+      </c>
+      <c r="S33" t="n">
+        <v>1.196184043816677</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.01727762707235645</v>
+      </c>
+      <c r="U33" t="n">
+        <v>1.249837675484804</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.0121196518451827</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.9612400134755495</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.0147855131470211</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.9327082563306478</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.01831031500975907</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0.9995909036625522</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0.01460121726061896</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.8902329439827643</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.01504363851998629</v>
       </c>
     </row>
     <row r="34">
@@ -2212,29 +3784,82 @@
           <t>[358.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>[Na,Cl]</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>[1,1]</t>
         </is>
       </c>
-      <c r="J34" t="b">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" t="n">
         <v>2482</v>
       </c>
-      <c r="L34" t="n">
+      <c r="M34" t="n">
         <v>1256254639</v>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="N34" t="inlineStr">
         <is>
           <t>test174_HPGe_2_Labr_4_Ing27_83prc_Generator_100hz_Ba_center_Pb_1mm_NaCl_4cm_pos0.root</t>
         </is>
+      </c>
+      <c r="O34" t="n">
+        <v>174</v>
+      </c>
+      <c r="P34" s="1" t="inlineStr">
+        <is>
+          <t>12/11/2024</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.6056408189657847</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.8698781465276079</v>
+      </c>
+      <c r="S34" t="n">
+        <v>1.409452015883075</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.01549387651419359</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1.202219303930534</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.02551416027851264</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.9864599997196395</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0.008397437077483413</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.9909221390840557</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0.01030196596674218</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>1.091532386404308</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0.01193065745257848</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0.9135333989277367</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0.01483127273628398</v>
       </c>
     </row>
     <row r="35">
@@ -2257,7 +3882,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[387.5,0,-7.5]</t>
+          <t>[391.5,0,-7.5]</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2265,29 +3890,82 @@
           <t>[376.0,0,-7.5]</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>[Fe]</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>[1]</t>
         </is>
       </c>
-      <c r="J35" t="b">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" t="n">
         <v>14400</v>
       </c>
-      <c r="L35" t="n">
+      <c r="M35" t="n">
         <v>8687557491</v>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="N35" t="inlineStr">
         <is>
           <t>test156_HPGe_2_Labr_4_Ing27_81prc_Generator_100hz_Ba_center_Pb_1mm_Fe_2cm.root</t>
         </is>
+      </c>
+      <c r="O35" t="n">
+        <v>156</v>
+      </c>
+      <c r="P35" s="1" t="inlineStr">
+        <is>
+          <t>08/08/2024</t>
+        </is>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.8506623983578424</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.8469682721740073</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1.441583366157438</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.01794770039657157</v>
+      </c>
+      <c r="U35" t="n">
+        <v>1.269211513967858</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.02294899917158088</v>
+      </c>
+      <c r="W35" t="n">
+        <v>1.08444640753837</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0.007173750943106289</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>1.035919736322347</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0.006888738583093983</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>1.068509460204027</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0.008021082853217201</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0.9979190144408214</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0.01206365156860205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>